<commit_message>
Atualização do relatório e cronograma
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>ATIVIDADES</t>
   </si>
@@ -42,20 +42,90 @@
     <t>Semana 14/05</t>
   </si>
   <si>
-    <t>Semana 21/05</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
     <t>2.1 Criação do rails server</t>
+  </si>
+  <si>
+    <t>2.0 Criação do first_app</t>
+  </si>
+  <si>
+    <t>X = Feito</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Não feito</t>
+    </r>
+  </si>
+  <si>
+    <t>3.0 Layout da página principal</t>
+  </si>
+  <si>
+    <t>Semana 28/05</t>
+  </si>
+  <si>
+    <t>2.4 Ligação entre usuário e postagem</t>
+  </si>
+  <si>
+    <t>4.0 Modelagem dos usuários</t>
+  </si>
+  <si>
+    <t>3.1 Criação dos arquivos .css</t>
+  </si>
+  <si>
+    <t>3.1.1 Botão "Cadastre-se"</t>
+  </si>
+  <si>
+    <t>3.1.2 Botão "Entrar"</t>
+  </si>
+  <si>
+    <t>4.1 Validação do usuário</t>
+  </si>
+  <si>
+    <t>4.2 Validação da senha</t>
+  </si>
+  <si>
+    <t>5.0 Formulário de inscrição</t>
+  </si>
+  <si>
+    <t>5.0.1 Criação de restrições do formulário</t>
+  </si>
+  <si>
+    <t>2.2 Sistema de cadastro</t>
+  </si>
+  <si>
+    <t>2.3  Sistema de postagem</t>
+  </si>
+  <si>
+    <t>Semana 04/06</t>
+  </si>
+  <si>
+    <t>Semana 11/06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -112,29 +182,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:F10" totalsRowShown="0">
-  <autoFilter ref="B3:F10">
-    <filterColumn colId="1"/>
-    <filterColumn colId="2"/>
-    <filterColumn colId="3"/>
-    <filterColumn colId="4"/>
-  </autoFilter>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B4:H24" totalsRowShown="0">
+  <autoFilter ref="B4:H24"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="ATIVIDADES"/>
     <tableColumn id="2" name="Semana 30/04"/>
     <tableColumn id="3" name="Semana 07/05"/>
     <tableColumn id="4" name="Semana 14/05"/>
-    <tableColumn id="5" name="Semana 21/05"/>
+    <tableColumn id="5" name="Semana 28/05"/>
+    <tableColumn id="6" name="Semana 04/06"/>
+    <tableColumn id="7" name="Semana 11/06"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -215,6 +291,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -249,6 +326,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -424,145 +502,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="59" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6">
-      <c r="B3" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="1" t="s">
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:6">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5" t="s">
-        <v>9</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="2:6">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="2:6">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:6">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="2:6">
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:6">
+      <c r="F14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:6">
+      <c r="F15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="F16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -574,24 +783,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Criação do história.txt e atualização do cronograma
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
@@ -124,8 +124,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,7 +291,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -326,7 +325,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -502,14 +500,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="59" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
@@ -521,17 +519,17 @@
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8">
       <c r="B1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8">
       <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -554,7 +552,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -565,7 +563,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -577,7 +575,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -589,7 +587,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -601,7 +599,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -613,7 +611,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -625,7 +623,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -637,7 +635,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -649,7 +647,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -662,46 +660,46 @@
       <c r="G13" s="5"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8">
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8">
       <c r="B15" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8">
       <c r="B16" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8">
       <c r="B17" t="s">
         <v>19</v>
       </c>
@@ -714,7 +712,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -727,7 +725,7 @@
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -740,7 +738,7 @@
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8">
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -753,7 +751,7 @@
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8">
       <c r="B21" t="s">
         <v>22</v>
       </c>
@@ -763,7 +761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -783,24 +781,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização do historia.txt e do cronograma
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>ATIVIDADES</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>Semana 11/06</t>
+  </si>
+  <si>
+    <t>Semana 18/07</t>
+  </si>
+  <si>
+    <t>6.0 Sign in e sign out da aplicação</t>
   </si>
 </sst>
 </file>
@@ -201,9 +207,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B4:H24" totalsRowShown="0">
-  <autoFilter ref="B4:H24"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B4:I24" totalsRowShown="0">
+  <autoFilter ref="B4:I24">
+    <filterColumn colId="7"/>
+  </autoFilter>
+  <tableColumns count="8">
     <tableColumn id="1" name="ATIVIDADES"/>
     <tableColumn id="2" name="Semana 30/04"/>
     <tableColumn id="3" name="Semana 07/05"/>
@@ -211,6 +219,7 @@
     <tableColumn id="5" name="Semana 28/05"/>
     <tableColumn id="6" name="Semana 04/06"/>
     <tableColumn id="7" name="Semana 11/06"/>
+    <tableColumn id="8" name="Semana 18/07"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -501,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H22"/>
+  <dimension ref="B1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -519,17 +528,17 @@
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8">
+    <row r="1" spans="2:9">
       <c r="B1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -551,8 +560,11 @@
       <c r="H4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="2:8">
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -563,7 +575,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -575,7 +587,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:9">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -587,7 +599,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -599,7 +611,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:9">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -611,7 +623,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:9">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -623,7 +635,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:9">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -635,7 +647,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:9">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -647,7 +659,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -660,7 +672,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:9">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -673,7 +685,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:9">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -686,7 +698,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:9">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -699,20 +711,20 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:9">
       <c r="B17" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -720,12 +732,12 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:9">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -733,12 +745,12 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -746,28 +758,36 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8">
+      <c r="H21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
       <c r="B22" t="s">
         <v>23</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>